<commit_message>
Correccion de Importes Informe Sigehos
</commit_message>
<xml_diff>
--- a/DBA/Reportes BI/2021/Facturación/Reporte DPH/Control-Sigehos.xlsx
+++ b/DBA/Reportes BI/2021/Facturación/Reporte DPH/Control-Sigehos.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t xml:space="preserve">EfectorSigehos</t>
   </si>
@@ -24,12 +24,6 @@
   </si>
   <si>
     <t xml:space="preserve">EfectorObjetivos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HOSP..DE.REHABILITACION.PSICOFISICA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IREP</t>
   </si>
 </sst>
 </file>
@@ -375,18 +369,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2"/>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>